<commit_message>
Created a few classes for the chart writing and refactored a bit to use them. Added some constants too
</commit_message>
<xml_diff>
--- a/gchart.xlsx
+++ b/gchart.xlsx
@@ -376,7 +376,7 @@
     <t>27 Virgo</t>
   </si>
   <si>
-    <t>Asc</t>
+    <t xml:space="preserve">28: [Asc] </t>
   </si>
   <si>
     <t>180</t>
@@ -421,7 +421,7 @@
     <t>18 Libra</t>
   </si>
   <si>
-    <t>Mars</t>
+    <t xml:space="preserve">19: [Mars] </t>
   </si>
   <si>
     <t>201</t>
@@ -430,7 +430,7 @@
     <t>21 Libra</t>
   </si>
   <si>
-    <t>Saturn</t>
+    <t xml:space="preserve">21: [Saturn] </t>
   </si>
   <si>
     <t>204</t>
@@ -439,7 +439,7 @@
     <t>24 Libra</t>
   </si>
   <si>
-    <t>Pluto</t>
+    <t xml:space="preserve">26: [Pluto] </t>
   </si>
   <si>
     <t>207</t>
@@ -472,7 +472,7 @@
     <t>9 Scorpio</t>
   </si>
   <si>
-    <t>Jupiter</t>
+    <t xml:space="preserve">10: [Jupiter] </t>
   </si>
   <si>
     <t>222</t>
@@ -523,7 +523,7 @@
     <t>3 Sagitarrius</t>
   </si>
   <si>
-    <t>Uranus</t>
+    <t xml:space="preserve">4: [Uranus] </t>
   </si>
   <si>
     <t>246</t>
@@ -568,7 +568,7 @@
     <t>24 Sagitarrius</t>
   </si>
   <si>
-    <t>Neptune</t>
+    <t xml:space="preserve">26: [Neptune] </t>
   </si>
   <si>
     <t>267</t>
@@ -613,7 +613,7 @@
     <t>15 Capricorn</t>
   </si>
   <si>
-    <t>Moon</t>
+    <t xml:space="preserve">17: [Moon] </t>
   </si>
   <si>
     <t>288</t>
@@ -634,7 +634,7 @@
     <t>24 Capricorn</t>
   </si>
   <si>
-    <t>Venus</t>
+    <t xml:space="preserve">25: [Venus] </t>
   </si>
   <si>
     <t>297</t>
@@ -655,7 +655,7 @@
     <t>3 Aquarius</t>
   </si>
   <si>
-    <t>Mercury</t>
+    <t xml:space="preserve">5: [Mercury] </t>
   </si>
   <si>
     <t>306</t>
@@ -712,7 +712,7 @@
     <t>0 Pisces</t>
   </si>
   <si>
-    <t>Sun</t>
+    <t xml:space="preserve">1: [Sun] </t>
   </si>
   <si>
     <t>333</t>

</xml_diff>